<commit_message>
Add messages per second
</commit_message>
<xml_diff>
--- a/benchmarks/compiled_benchmarks.xlsx
+++ b/benchmarks/compiled_benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joonas\Documents\Yliopisto\Scalable-Systems-and-Data-Management-Project-CS-E4780\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB107C2D-0498-4765-8D05-289CB7AF2400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8BEB21-7D1F-4626-A123-931A75496CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{2FA3B4F8-90A2-4D90-A3A2-612E125FA6F2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Joonas PC</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Luan laptop</t>
+  </si>
+  <si>
+    <t>Messages_per_second</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -118,48 +128,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5CA54E7E-0002-49E5-ADA3-8485CE68A938}" name="Table1" displayName="Table1" ref="A2:E17" totalsRowShown="0">
-  <autoFilter ref="A2:E17" xr:uid="{5CA54E7E-0002-49E5-ADA3-8485CE68A938}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5CA54E7E-0002-49E5-ADA3-8485CE68A938}" name="Table1" displayName="Table1" ref="A2:F17" totalsRowShown="0">
+  <autoFilter ref="A2:F17" xr:uid="{5CA54E7E-0002-49E5-ADA3-8485CE68A938}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CCEC4A68-3782-44B9-9C5F-876DB4C8923E}" name="workers"/>
     <tableColumn id="2" xr3:uid="{C45DAD5F-C225-4011-A947-4700F4032C9F}" name="simulators"/>
     <tableColumn id="3" xr3:uid="{F392C65C-D41C-4EAE-9A86-3A43A9EA08AD}" name="events"/>
     <tableColumn id="4" xr3:uid="{FA27454D-9057-4CF1-969C-9F45CDDA6C56}" name="events_percentage">
-      <calculatedColumnFormula>C3/(B3*$S$2) * 100</calculatedColumnFormula>
+      <calculatedColumnFormula>C3/(B3*$V$2) * 100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{DC2A8159-639B-4C29-86F4-5FFA71B02A4E}" name="latency"/>
+    <tableColumn id="6" xr3:uid="{20B13B07-7188-4288-A5EE-2040615B6A5F}" name="Messages_per_second" dataDxfId="1">
+      <calculatedColumnFormula>B3*1000000*3 / 300</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE90AA53-0523-49A7-AEF1-92DBE6CDE110}" name="Table2" displayName="Table2" ref="G2:K22" totalsRowShown="0">
-  <autoFilter ref="G2:K22" xr:uid="{FE90AA53-0523-49A7-AEF1-92DBE6CDE110}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE90AA53-0523-49A7-AEF1-92DBE6CDE110}" name="Table2" displayName="Table2" ref="H2:M22" totalsRowShown="0">
+  <autoFilter ref="H2:M22" xr:uid="{FE90AA53-0523-49A7-AEF1-92DBE6CDE110}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6B15D70F-3872-4520-80A2-4681F3FD0917}" name="workers"/>
     <tableColumn id="2" xr3:uid="{8F8A57CF-97D5-4F12-80F6-E2B7BF59DE86}" name="simulators"/>
     <tableColumn id="3" xr3:uid="{36108E73-215A-4C55-AAA5-387026B51159}" name="events"/>
     <tableColumn id="4" xr3:uid="{5605A464-D98A-40DE-BFD2-46CB8296EABC}" name="events_percentage">
-      <calculatedColumnFormula>I3/(H3*$S$2) * 100</calculatedColumnFormula>
+      <calculatedColumnFormula>J3/(I3*$V$2) * 100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{CD645A99-9C76-4AE2-A112-9AE3CC68ABD8}" name="latency"/>
+    <tableColumn id="6" xr3:uid="{5CADFE77-65AE-4521-B355-5897C59C26F3}" name="Messages_per_second" dataDxfId="0">
+      <calculatedColumnFormula>I3*1000000*3 / 300</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4EF5E628-066B-4A8E-BC96-29EDE94C93C5}" name="Table3" displayName="Table3" ref="M2:Q17" totalsRowShown="0">
-  <autoFilter ref="M2:Q17" xr:uid="{4EF5E628-066B-4A8E-BC96-29EDE94C93C5}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4EF5E628-066B-4A8E-BC96-29EDE94C93C5}" name="Table3" displayName="Table3" ref="O2:T17" totalsRowShown="0">
+  <autoFilter ref="O2:T17" xr:uid="{4EF5E628-066B-4A8E-BC96-29EDE94C93C5}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CAA8B1A0-9ECC-4A33-9E2F-7CEC1A8203DF}" name="workers"/>
     <tableColumn id="2" xr3:uid="{99853473-CE9D-40E5-845B-12AB0D3204C3}" name="simulators"/>
     <tableColumn id="3" xr3:uid="{027A90E0-AF38-4518-B2C5-7BEC1058C481}" name="events"/>
     <tableColumn id="4" xr3:uid="{319CCE17-707B-4028-B0AE-B3C51AE80006}" name="events_percentage">
-      <calculatedColumnFormula>O3/(N3*$S$2) * 100</calculatedColumnFormula>
+      <calculatedColumnFormula>Q3/(P3*$V$2) * 100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{7969A7F7-EF87-4286-A1E1-1DC660123657}" name="latency"/>
+    <tableColumn id="6" xr3:uid="{3AF15C0D-8B01-4B6E-B78C-5E771EE14501}" name="Messages_per_second">
+      <calculatedColumnFormula>P3*1000000*3 / 300</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,48 +501,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B568AEB-71B0-4754-9C06-117CF1C56E6B}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" customWidth="1"/>
-    <col min="19" max="19" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -539,42 +563,51 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>4</v>
       </c>
-      <c r="S2">
+      <c r="T2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2">
         <f>899994</f>
         <v>899994</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -585,46 +618,58 @@
         <v>899994</v>
       </c>
       <c r="D3">
-        <f>C3/(B3*$S$2) * 100</f>
+        <f>C3/(B3*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E3">
         <v>552</v>
       </c>
-      <c r="G3">
-        <v>1</v>
+      <c r="F3">
+        <f t="shared" ref="F3:F17" si="0">B3*1000000*3 / 300</f>
+        <v>10000</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>899994</v>
       </c>
-      <c r="J3">
-        <f>I3/(H3*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K3">
+        <f>J3/(I3*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L3">
         <v>508</v>
       </c>
       <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
+        <f t="shared" ref="M3:M22" si="1">I3*1000000*3 / 300</f>
+        <v>10000</v>
       </c>
       <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>899994</v>
       </c>
-      <c r="P3">
-        <f>O3/(N3*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q3">
+      <c r="R3">
+        <f>Q3/(P3*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S3">
         <v>526</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <f t="shared" ref="T3:T17" si="2">P3*1000000*3 / 300</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -635,46 +680,58 @@
         <v>899994</v>
       </c>
       <c r="D4">
-        <f>C4/(B4*$S$2) * 100</f>
+        <f>C4/(B4*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E4">
         <v>540</v>
       </c>
-      <c r="G4">
-        <v>2</v>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>10000</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>899994</v>
       </c>
-      <c r="J4">
-        <f>I4/(H4*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K4">
+        <f>J4/(I4*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L4">
         <v>551</v>
       </c>
       <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>10000</v>
       </c>
       <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>899994</v>
       </c>
-      <c r="P4">
-        <f>O4/(N4*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q4">
+      <c r="R4">
+        <f>Q4/(P4*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S4">
         <v>521</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -685,46 +742,58 @@
         <v>899994</v>
       </c>
       <c r="D5">
-        <f>C5/(B5*$S$2) * 100</f>
+        <f>C5/(B5*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E5">
         <v>521</v>
       </c>
-      <c r="G5">
-        <v>3</v>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>10000</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>899994</v>
       </c>
-      <c r="J5">
-        <f>I5/(H5*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K5">
+        <f>J5/(I5*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L5">
         <v>473</v>
       </c>
       <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>10000</v>
       </c>
       <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>899994</v>
       </c>
-      <c r="P5">
-        <f>O5/(N5*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q5">
+      <c r="R5">
+        <f>Q5/(P5*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S5">
         <v>535</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -735,46 +804,58 @@
         <v>1799988</v>
       </c>
       <c r="D6">
-        <f>C6/(B6*$S$2) * 100</f>
+        <f>C6/(B6*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E6">
         <v>585</v>
       </c>
-      <c r="G6">
-        <v>1</v>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>20000</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
         <v>1799988</v>
       </c>
-      <c r="J6">
-        <f>I6/(H6*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K6">
+        <f>J6/(I6*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L6">
         <v>502</v>
       </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>20000</v>
       </c>
       <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
         <v>1799988</v>
       </c>
-      <c r="P6">
-        <f>O6/(N6*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q6">
+      <c r="R6">
+        <f>Q6/(P6*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S6">
         <v>557</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -785,46 +866,58 @@
         <v>1799988</v>
       </c>
       <c r="D7">
-        <f>C7/(B7*$S$2) * 100</f>
+        <f>C7/(B7*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E7">
         <v>566</v>
       </c>
-      <c r="G7">
-        <v>2</v>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>20000</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>1799988</v>
       </c>
-      <c r="J7">
-        <f>I7/(H7*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K7">
+        <f>J7/(I7*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L7">
         <v>477</v>
       </c>
       <c r="M7">
-        <v>2</v>
-      </c>
-      <c r="N7">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>20000</v>
       </c>
       <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
         <v>1799988</v>
       </c>
-      <c r="P7">
-        <f>O7/(N7*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q7">
+      <c r="R7">
+        <f>Q7/(P7*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S7">
         <v>527</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -835,46 +928,58 @@
         <v>1799988</v>
       </c>
       <c r="D8">
-        <f>C8/(B8*$S$2) * 100</f>
+        <f>C8/(B8*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E8">
         <v>538</v>
       </c>
-      <c r="G8">
-        <v>3</v>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>20000</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
         <v>1799988</v>
       </c>
-      <c r="J8">
-        <f>I8/(H8*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K8">
+        <f>J8/(I8*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L8">
         <v>517</v>
       </c>
       <c r="M8">
-        <v>3</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>20000</v>
       </c>
       <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
         <v>1799988</v>
       </c>
-      <c r="P8">
-        <f>O8/(N8*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q8">
+      <c r="R8">
+        <f>Q8/(P8*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S8">
         <v>525</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -885,46 +990,58 @@
         <v>1646560</v>
       </c>
       <c r="D9">
-        <f>C9/(B9*$S$2) * 100</f>
+        <f>C9/(B9*$V$2) * 100</f>
         <v>60.984110264438797</v>
       </c>
       <c r="E9">
         <v>1480</v>
       </c>
-      <c r="G9">
-        <v>1</v>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>30000</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
         <v>2699982</v>
       </c>
-      <c r="J9">
-        <f>I9/(H9*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K9">
+        <f>J9/(I9*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L9">
         <v>525</v>
       </c>
       <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>30000</v>
       </c>
       <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
         <v>2024287</v>
       </c>
-      <c r="P9">
-        <f>O9/(N9*$S$2) * 100</f>
+      <c r="R9">
+        <f>Q9/(P9*$V$2) * 100</f>
         <v>74.97409241987539</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>1450</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -935,46 +1052,58 @@
         <v>2376571</v>
       </c>
       <c r="D10">
-        <f>C10/(B10*$S$2) * 100</f>
+        <f>C10/(B10*$V$2) * 100</f>
         <v>88.02173495971455</v>
       </c>
       <c r="E10">
         <v>1630</v>
       </c>
-      <c r="G10">
-        <v>2</v>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>30000</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
         <v>2699982</v>
       </c>
-      <c r="J10">
-        <f>I10/(H10*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K10">
+        <f>J10/(I10*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L10">
         <v>542</v>
       </c>
       <c r="M10">
-        <v>2</v>
-      </c>
-      <c r="N10">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>30000</v>
       </c>
       <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
         <v>2699982</v>
       </c>
-      <c r="P10">
-        <f>O10/(N10*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q10">
+      <c r="R10">
+        <f>Q10/(P10*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S10">
         <v>530</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -985,46 +1114,58 @@
         <v>2699982</v>
       </c>
       <c r="D11">
-        <f>C11/(B11*$S$2) * 100</f>
+        <f>C11/(B11*$V$2) * 100</f>
         <v>100</v>
       </c>
       <c r="E11">
         <v>716</v>
       </c>
-      <c r="G11">
-        <v>3</v>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>30000</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
       <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
         <v>2699982</v>
       </c>
-      <c r="J11">
-        <f>I11/(H11*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K11">
+        <f>J11/(I11*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L11">
         <v>516</v>
       </c>
       <c r="M11">
-        <v>3</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>30000</v>
       </c>
       <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11">
         <v>2699982</v>
       </c>
-      <c r="P11">
-        <f>O11/(N11*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q11">
+      <c r="R11">
+        <f>Q11/(P11*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S11">
         <v>525</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1035,46 +1176,58 @@
         <v>1609225</v>
       </c>
       <c r="D12">
-        <f>C12/(B12*$S$2) * 100</f>
+        <f>C12/(B12*$V$2) * 100</f>
         <v>44.700992451060785</v>
       </c>
       <c r="E12">
         <v>1330</v>
       </c>
-      <c r="G12">
-        <v>1</v>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>40000</v>
       </c>
       <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>4</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>3599976</v>
       </c>
-      <c r="J12">
-        <f>I12/(H12*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K12">
+        <f>J12/(I12*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L12">
         <v>528</v>
       </c>
       <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
         <v>4</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>1804176</v>
       </c>
-      <c r="P12">
-        <f>O12/(N12*$S$2) * 100</f>
+      <c r="R12">
+        <f>Q12/(P12*$V$2) * 100</f>
         <v>50.116334108894058</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>1100</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1085,46 +1238,58 @@
         <v>2528755</v>
       </c>
       <c r="D13">
-        <f>C13/(B13*$S$2) * 100</f>
+        <f>C13/(B13*$V$2) * 100</f>
         <v>70.243662735529341</v>
       </c>
       <c r="E13">
         <v>1490</v>
       </c>
-      <c r="G13">
-        <v>2</v>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>40000</v>
       </c>
       <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>4</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>3599976</v>
       </c>
-      <c r="J13">
-        <f>I13/(H13*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K13">
+        <f>J13/(I13*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L13">
         <v>504</v>
       </c>
       <c r="M13">
-        <v>2</v>
-      </c>
-      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
         <v>4</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>3343420</v>
       </c>
-      <c r="P13">
-        <f>O13/(N13*$S$2) * 100</f>
+      <c r="R13">
+        <f>Q13/(P13*$V$2) * 100</f>
         <v>92.873396933757334</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>1260</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1135,46 +1300,58 @@
         <v>3217078</v>
       </c>
       <c r="D14">
-        <f>C14/(B14*$S$2) * 100</f>
+        <f>C14/(B14*$V$2) * 100</f>
         <v>89.36387353693469</v>
       </c>
       <c r="E14">
         <v>1540</v>
       </c>
-      <c r="G14">
-        <v>3</v>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>40000</v>
       </c>
       <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
         <v>4</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>3599976</v>
       </c>
-      <c r="J14">
-        <f>I14/(H14*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K14">
+        <f>J14/(I14*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L14">
         <v>504</v>
       </c>
       <c r="M14">
-        <v>3</v>
-      </c>
-      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
         <v>4</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>3599976</v>
       </c>
-      <c r="P14">
-        <f>O14/(N14*$S$2) * 100</f>
-        <v>100</v>
-      </c>
-      <c r="Q14">
+      <c r="R14">
+        <f>Q14/(P14*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="S14">
         <v>532</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1185,46 +1362,58 @@
         <v>1838368</v>
       </c>
       <c r="D15">
-        <f>C15/(B15*$S$2) * 100</f>
+        <f>C15/(B15*$V$2) * 100</f>
         <v>40.852894574852719</v>
       </c>
       <c r="E15">
         <v>1330</v>
       </c>
-      <c r="G15">
-        <v>1</v>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>50000</v>
       </c>
       <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>5</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>4499970</v>
       </c>
-      <c r="J15">
-        <f>I15/(H15*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K15">
+        <f>J15/(I15*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L15">
         <v>663</v>
       </c>
       <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
         <v>5</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>1794472</v>
       </c>
-      <c r="P15">
-        <f>O15/(N15*$S$2) * 100</f>
+      <c r="R15">
+        <f>Q15/(P15*$V$2) * 100</f>
         <v>39.87742140503159</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>1100</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1235,46 +1424,58 @@
         <v>2937143</v>
       </c>
       <c r="D16">
-        <f>C16/(B16*$S$2) * 100</f>
+        <f>C16/(B16*$V$2) * 100</f>
         <v>65.270279579641638</v>
       </c>
       <c r="E16">
         <v>1480</v>
       </c>
-      <c r="G16">
-        <v>2</v>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>50000</v>
       </c>
       <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
         <v>5</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>4499970</v>
       </c>
-      <c r="J16">
-        <f>I16/(H16*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K16">
+        <f>J16/(I16*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L16">
         <v>539</v>
       </c>
       <c r="M16">
-        <v>2</v>
-      </c>
-      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
         <v>5</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>3398343</v>
       </c>
-      <c r="P16">
-        <f>O16/(N16*$S$2) * 100</f>
+      <c r="R16">
+        <f>Q16/(P16*$V$2) * 100</f>
         <v>75.519236794911976</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>1170</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1285,133 +1486,165 @@
         <v>3795566</v>
       </c>
       <c r="D17">
-        <f>C17/(B17*$S$2) * 100</f>
+        <f>C17/(B17*$V$2) * 100</f>
         <v>84.346473420933918</v>
       </c>
       <c r="E17">
         <v>1540</v>
       </c>
-      <c r="G17">
-        <v>3</v>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>50000</v>
       </c>
       <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
         <v>5</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>4499970</v>
       </c>
-      <c r="J17">
-        <f>I17/(H17*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K17">
+        <f>J17/(I17*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L17">
         <v>521</v>
       </c>
       <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="P17">
         <v>5</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>4169089</v>
       </c>
-      <c r="P17">
-        <f>O17/(N17*$S$2) * 100</f>
+      <c r="R17">
+        <f>Q17/(P17*$V$2) * 100</f>
         <v>92.647039869154682</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>1190</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G18">
-        <v>1</v>
-      </c>
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>6</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>5104365</v>
       </c>
-      <c r="J18">
-        <f>I18/(H18*$S$2) * 100</f>
+      <c r="K18">
+        <f>J18/(I18*$V$2) * 100</f>
         <v>94.525907950497441</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>900</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G19">
-        <v>2</v>
-      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
         <v>6</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>5399964</v>
       </c>
-      <c r="J19">
-        <f>I19/(H19*$S$2) * 100</f>
-        <v>100</v>
-      </c>
       <c r="K19">
+        <f>J19/(I19*$V$2) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="L19">
         <v>538</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G20">
-        <v>2</v>
-      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
         <v>7</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>5988192</v>
       </c>
-      <c r="J20">
-        <f>I20/(H20*$S$2) * 100</f>
+      <c r="K20">
+        <f>J20/(I20*$V$2) * 100</f>
         <v>95.051300342002278</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>923</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G21">
-        <v>2</v>
-      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
         <v>8</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>6448528</v>
       </c>
-      <c r="J21">
-        <f>I21/(H21*$S$2) * 100</f>
+      <c r="K21">
+        <f>J21/(I21*$V$2) * 100</f>
         <v>89.563485978795413</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>850</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G22">
-        <v>3</v>
-      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
         <v>7</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>6172881</v>
       </c>
-      <c r="J22">
-        <f>I22/(H22*$S$2) * 100</f>
+      <c r="K22">
+        <f>J22/(I22*$V$2) * 100</f>
         <v>97.982891314513523</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>768</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>70000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>